<commit_message>
Atualização automática de GIRUA.xlsx
</commit_message>
<xml_diff>
--- a/GIRUA.xlsx
+++ b/GIRUA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0646F7-1109-43DC-A4AD-7B7884541680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43180659-B8F2-4D7C-A4F8-C8E9420B56EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -993,7 +993,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1053,36 +1053,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1116,14 +1092,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1140,7 +1112,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1155,7 +1126,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{CABE7163-9875-4AA9-8869-C650ED92F9A8}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{6A18AE50-F243-4118-95DA-6178422D3480}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1185,10 +1156,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCEBBF0-EF2E-45D3-8635-501DB46E120C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF0C9326-4DC6-4ED9-9451-2CDBB822844F}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1226,7 +1197,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3980893-E14B-41EF-AA67-F0B1D46974EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DC0E055-5600-4EDF-8F7C-3D10E93E233B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1289,7 +1260,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18854780-49AC-421F-B776-A853722F053F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DE16469-7286-423C-A253-121DEECA3978}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1308,7 +1279,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE83A39-4B7A-0718-ED55-1AA2397E212C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB539D4-7816-F5D7-3E3D-BC32EE3A80C0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1357,7 +1328,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7748F4A6-6F97-51E2-2205-BFBFD5B67C47}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C35F23-FFB4-7B74-52FD-C060EB809FDD}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1376,7 +1347,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6B3FCB-ACF3-049C-BC9D-B7FA1D319AD1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E685FA-BF18-69FC-B219-105024CB8B5D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1407,7 +1378,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D8E788-8E91-694C-0C8E-053DC81920CE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{515FB7DE-69EE-068C-9AE9-7CA0B0D7056F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1438,7 +1409,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEEC7C4A-4E8A-D329-719F-08DCC52DCE21}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76E3133D-59E9-B6C3-0FBD-518E79A1FE5E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1481,7 +1452,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB5FD35-86D8-4EDE-BCC5-9023F6A58EBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{863D978C-14B5-4CC4-AE9D-27970C55A43C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1519,7 +1490,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{498A9355-E3D0-4D38-B7F5-AC027F244504}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38BC902D-62FE-4557-B037-70D8BC7025A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,7 +1533,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCEC56E2-4E7A-46EA-AFDD-EA06DFF91577}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A513F292-7327-4048-83CE-3032AB5B3FE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1875,7 +1846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A4EE93-C326-4D6E-85E7-6FDADA2486FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67D0CF1-66B2-4A21-BD1D-A59D4A79683A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1887,98 +1858,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="30"/>
-    <col min="6" max="6" width="2" style="30" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="30" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="30"/>
+    <col min="1" max="5" width="12.5703125" style="27"/>
+    <col min="6" max="6" width="2" style="27" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="27" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="29"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="29"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="29"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="29"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="29"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="29"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="29"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="29"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="29"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="29"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="29"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="29"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="29"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="29"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="29"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="29"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="29"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="29"/>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="29"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="29"/>
+      <c r="F20" s="26"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="29"/>
+      <c r="F21" s="26"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="29"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="29"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="29"/>
+      <c r="F24" s="26"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="29"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="29"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="29"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="29"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="29"/>
+      <c r="F29" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5125,19 +5096,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5160,46 +5131,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5224,99 +5195,100 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="18" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="21">
         <v>45839</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="23">
         <v>7756</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="23">
         <v>1381</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="25" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>